<commit_message>
Updated CCED and Sustainability
</commit_message>
<xml_diff>
--- a/DOCS/CCED_Metric.xlsx
+++ b/DOCS/CCED_Metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Desktop\Lewis\Year 4 - Semester 2\Software Systems Capstone\Software-Systems-Capstone\UltimateSeatSelector\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4749ED68-728A-4E07-A6AF-928ECCD38F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E586F0-FB1A-4F90-B591-FF0E3AD13FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint5" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -89,16 +89,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>EJP</t>
-  </si>
-  <si>
     <t>Eric Pogue</t>
   </si>
   <si>
     <t>James Pogue</t>
-  </si>
-  <si>
-    <t>JP</t>
   </si>
   <si>
     <t>Preliminary Signoff</t>
@@ -108,18 +102,6 @@
   </si>
   <si>
     <t>Date/Time</t>
-  </si>
-  <si>
-    <t>January 29, 2023 @ 11:58 pm</t>
-  </si>
-  <si>
-    <t>January 29, 2023 @ 11:59 pm</t>
-  </si>
-  <si>
-    <t>January 30, 2023 @ 2:06 pm</t>
-  </si>
-  <si>
-    <t>January 30, 2023 @ 2:07 pm</t>
   </si>
   <si>
     <t>Team Eric's Angels</t>
@@ -153,6 +135,9 @@
   </si>
   <si>
     <t>April 23, 2023 @ 10:11 pm</t>
+  </si>
+  <si>
+    <t>May 3, 2023 @ 12:46 pm</t>
   </si>
 </sst>
 </file>
@@ -535,7 +520,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
@@ -551,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -567,7 +552,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -578,7 +563,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -619,7 +604,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9" s="7">
         <v>14</v>
@@ -649,7 +634,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B10" s="7">
         <v>14</v>
@@ -679,7 +664,7 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
       <c r="A11" s="20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7">
         <v>14</v>
@@ -766,14 +751,14 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -782,11 +767,11 @@
         <v>12</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -795,11 +780,11 @@
         <v>13</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E18" s="7"/>
     </row>
@@ -811,7 +796,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>14</v>
@@ -6809,7 +6794,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -6820,7 +6805,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -7011,14 +6996,14 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -7027,11 +7012,11 @@
         <v>12</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -7052,7 +7037,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>14</v>
@@ -13003,7 +12988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22623D9-D265-E341-9D40-D4F8180816A9}">
   <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -13055,7 +13040,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -13066,7 +13051,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -13257,14 +13242,14 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -13273,11 +13258,11 @@
         <v>12</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -13298,7 +13283,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>14</v>
@@ -19247,10 +19232,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE28E1FE-DF56-8B47-AF8A-1EC59E1B4672}">
-  <dimension ref="A1:I1008"/>
+  <dimension ref="A1:I1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -19301,7 +19286,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -19312,7 +19297,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -19370,7 +19355,7 @@
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9">
-        <f t="shared" ref="G9:H14" si="0">D9/B9</f>
+        <f t="shared" ref="G9:H11" si="0">D9/B9</f>
         <v>1</v>
       </c>
       <c r="H9" s="10">
@@ -19378,7 +19363,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="10">
-        <f t="shared" ref="I9:I16" si="1">E9/B9</f>
+        <f t="shared" ref="I9:I13" si="1">E9/B9</f>
         <v>1</v>
       </c>
     </row>
@@ -19388,16 +19373,16 @@
         <v>Connor Thompson</v>
       </c>
       <c r="B10" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C10" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D10" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E10" s="7">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9">
@@ -19445,60 +19430,43 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A12" s="11" t="e">
-        <f>Sprint5!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A13" s="11" t="e">
-        <f>Sprint5!#REF!</f>
-        <v>#REF!</v>
+      <c r="A13" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="B13" s="7">
-        <v>1</v>
+        <f>SUM(B9:B11)</f>
+        <v>14</v>
       </c>
       <c r="C13" s="7">
-        <v>1</v>
+        <f>SUM(C9:C11)</f>
+        <v>14</v>
       </c>
       <c r="D13" s="7">
-        <v>1</v>
+        <f>SUM(D9:D11)</f>
+        <v>14</v>
       </c>
       <c r="E13" s="7">
-        <v>1</v>
+        <f>SUM(E9:E11)</f>
+        <v>14</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G13:H13" si="2">D13/B13</f>
         <v>1</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I13" s="10">
@@ -19507,209 +19475,141 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="e">
-        <f>Sprint5!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="7">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>8</v>
+      <c r="A16" s="14" t="s">
+        <v>18</v>
       </c>
-      <c r="B16" s="7">
-        <f>SUM(B9:B14)</f>
-        <v>6</v>
+      <c r="B16" s="15" t="s">
+        <v>14</v>
       </c>
-      <c r="C16" s="7">
-        <f>SUM(C9:C14)</f>
-        <v>6</v>
-      </c>
-      <c r="D16" s="7">
-        <f>SUM(D9:D14)</f>
-        <v>6</v>
-      </c>
-      <c r="E16" s="7">
-        <f>SUM(E9:E14)</f>
-        <v>6</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9">
-        <f t="shared" ref="G16:H16" si="2">D16/B16</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A19" s="14" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14" t="s">
-        <v>22</v>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>15</v>
       </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A20" s="11" t="s">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>19</v>
+      <c r="B21" s="16" t="s">
+        <v>25</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="7"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="3"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="7"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="B29" s="3"/>
@@ -25573,24 +25473,6 @@
       <c r="D1005" s="3"/>
       <c r="E1005" s="3"/>
     </row>
-    <row r="1006" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B1006" s="3"/>
-      <c r="C1006" s="3"/>
-      <c r="D1006" s="3"/>
-      <c r="E1006" s="3"/>
-    </row>
-    <row r="1007" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B1007" s="3"/>
-      <c r="C1007" s="3"/>
-      <c r="D1007" s="3"/>
-      <c r="E1007" s="3"/>
-    </row>
-    <row r="1008" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B1008" s="3"/>
-      <c r="C1008" s="3"/>
-      <c r="D1008" s="3"/>
-      <c r="E1008" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>